<commit_message>
Updates to module 6
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_6.xlsx
+++ b/templates/NHWA_Module_6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\EST\Excel_Data_Importer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533A79CA-DAAA-4778-A3CC-889B5E364217}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E039DA3-8173-4CB0-A753-E11D38B37EAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DNn2ED2tvDz8R2HdUrc6XR6aLxi7PHt3jXYcZD0jxFrPsDBA7xDhVMdxOKshsbgCwgXdklO6j3XC0t5iHKIwCg==" workbookSaltValue="hoPvbRWBNZzUUX5QAUaMpQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -2762,6 +2762,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2781,8 +2784,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2794,22 +2803,13 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2818,16 +2818,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -4032,20 +4031,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -4072,20 +4071,20 @@
       </c>
     </row>
     <row r="2" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="45" t="s">
         <v>768</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -4257,16 +4256,16 @@
       </c>
     </row>
     <row r="6" spans="2:31" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="47" t="s">
         <v>763</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="52" t="s">
         <v>788</v>
       </c>
-      <c r="E6" s="61"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -4277,11 +4276,11 @@
       <c r="M6" s="2"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
       <c r="Y6" s="4" t="s">
         <v>16</v>
       </c>
@@ -4308,10 +4307,10 @@
       </c>
     </row>
     <row r="7" spans="2:31" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="61"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -4359,7 +4358,7 @@
       <c r="C8" s="17" t="s">
         <v>769</v>
       </c>
-      <c r="D8" s="60"/>
+      <c r="D8" s="61"/>
       <c r="E8" s="62"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -4492,22 +4491,22 @@
       </c>
     </row>
     <row r="11" spans="2:31" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="48" t="s">
         <v>787</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="49" t="s">
         <v>789</v>
       </c>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="42" t="s">
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="43" t="s">
         <v>790</v>
       </c>
       <c r="N11" s="14"/>
@@ -4543,9 +4542,9 @@
       </c>
     </row>
     <row r="12" spans="2:31" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="48"/>
       <c r="E12" s="24" t="s">
         <v>775</v>
       </c>
@@ -4558,7 +4557,7 @@
       <c r="H12" s="24" t="s">
         <v>786</v>
       </c>
-      <c r="I12" s="43"/>
+      <c r="I12" s="44"/>
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
@@ -10904,7 +10903,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="k5WLaYVqQv4j6zpGYXQVhwccn5iD/wlID+cnpmcDkZq05rPeEJ5OltkYc+nENGaAESsICF85rEADnGjgFcOklg==" saltValue="Y0UpyvBZGiBCYwWrcKtcww==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="TrFa5rq1hXR/BpZFDHt5kKOCzZFbXrDOSEQB2N0Sqh7LzjCStbsQ4vP82XXgeceS02zaUqX23KzyylVXQqJStw==" saltValue="2h6KEJ4rVQTADc4W/wfx6g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="I4 Q8:R15 J13:M19 N8:P14" name="Range1"/>
     <protectedRange sqref="F13:I19 D13:E16 D18:E19" name="Range1_1"/>
@@ -10992,36 +10991,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
     </row>
     <row r="2" spans="2:19" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="45" t="s">
         <v>768</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
       <c r="N2" s="11" t="e">
         <f>Characteristics!V2</f>
         <v>#N/A</v>
@@ -11086,33 +11085,33 @@
       </c>
     </row>
     <row r="7" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="47" t="s">
         <v>770</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="57" t="s">
         <v>771</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="47" t="s">
         <v>773</v>
       </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
       <c r="N7" s="11" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
       <c r="O8" s="11"/>
       <c r="P8" s="4" t="s">
         <v>765</v>
@@ -11135,10 +11134,10 @@
         <v>791</v>
       </c>
       <c r="D9" s="29"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
       <c r="N9" s="11">
         <v>1</v>
       </c>
@@ -11164,10 +11163,10 @@
         <v>792</v>
       </c>
       <c r="D10" s="29"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
       <c r="N10" s="11">
         <v>1</v>
       </c>
@@ -11189,10 +11188,10 @@
         <v>793</v>
       </c>
       <c r="D11" s="32"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
       <c r="N11" s="11">
         <v>1</v>
       </c>
@@ -11212,16 +11211,16 @@
       <c r="D12" s="39"/>
     </row>
     <row r="14" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="47" t="s">
         <v>770</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="55" t="s">
         <v>775</v>
       </c>
-      <c r="E14" s="55" t="s">
+      <c r="E14" s="57" t="s">
         <v>776</v>
       </c>
       <c r="F14" s="58"/>
@@ -11229,9 +11228,9 @@
       <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="57"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="56"/>
       <c r="E15" s="23" t="s">
         <v>777</v>
       </c>
@@ -11297,6 +11296,12 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="njO8t2UNzwLibFRM7/QfgGWZVKVcn/gHeiCHWwDTPFdW/Pju/K7pTCpOKjHRfrbNCcEYYzPWr9IIT7bp2ycbTQ==" saltValue="rbWw0nActd2GAs+GRzK7kw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="13">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="E7:H8"/>
     <mergeCell ref="E9:H9"/>
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="E11:H11"/>
@@ -11304,12 +11309,6 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:H14"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="E7:H8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:H16 E19:H20" xr:uid="{BB8CFBDE-3701-4918-8149-6D661D113196}">
@@ -11417,32 +11416,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="2:18" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="45" t="s">
         <v>768</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -11508,22 +11507,22 @@
       </c>
     </row>
     <row r="7" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="48" t="s">
         <v>794</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="48" t="s">
         <v>773</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
       <c r="M7" s="4" t="s">
         <v>766</v>
       </c>
@@ -11532,14 +11531,14 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
       <c r="O8" s="11"/>
       <c r="P8" s="4" t="s">
         <v>765</v>
@@ -11559,11 +11558,11 @@
         <v>4</v>
       </c>
       <c r="D9" s="21"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
       <c r="N9" s="11">
         <v>1</v>
       </c>
@@ -11589,11 +11588,11 @@
         <v>782</v>
       </c>
       <c r="D10" s="21"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
       <c r="N10" s="11">
         <v>1</v>
       </c>
@@ -11619,11 +11618,11 @@
         <v>783</v>
       </c>
       <c r="D11" s="21"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
       <c r="N11" s="11">
         <v>1</v>
       </c>
@@ -11649,11 +11648,11 @@
         <v>5</v>
       </c>
       <c r="D12" s="21"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
       <c r="N12" s="11">
         <v>1</v>
       </c>
@@ -11679,11 +11678,11 @@
         <v>6</v>
       </c>
       <c r="D13" s="21"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
       <c r="N13" s="11">
         <v>1</v>
       </c>
@@ -11709,11 +11708,11 @@
         <v>7</v>
       </c>
       <c r="D14" s="21"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
       <c r="N14" s="11">
         <v>1</v>
       </c>
@@ -11739,11 +11738,11 @@
         <v>8</v>
       </c>
       <c r="D15" s="21"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
       <c r="N15" s="11">
         <v>1</v>
       </c>
@@ -11770,34 +11769,34 @@
       <c r="O17" s="11"/>
     </row>
     <row r="18" spans="2:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="60" t="s">
         <v>763</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="55" t="s">
         <v>764</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="47" t="s">
         <v>773</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
     </row>
     <row r="19" spans="2:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="46"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
     </row>
@@ -11809,11 +11808,11 @@
         <v>795</v>
       </c>
       <c r="D20" s="21"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
       <c r="N20" s="11">
         <v>1</v>
       </c>
@@ -11830,11 +11829,11 @@
         <v>796</v>
       </c>
       <c r="D21" s="21"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
       <c r="N21" s="11">
         <v>1</v>
       </c>
@@ -11855,6 +11854,9 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="U6zHl81zHEJFHtcGEmWN7K/Nl7VQXEMwqrV3P/k+2/k78IMzbhKEqDtEEXpRJWX9nJ1s2RpNkh1Lzmte3WBCkg==" saltValue="maxO/YNHiX/BdQ39wuXx1g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="19">
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E18:I19"/>
+    <mergeCell ref="E20:I20"/>
     <mergeCell ref="E21:I21"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="B1:I1"/>
@@ -11871,9 +11873,6 @@
     <mergeCell ref="E12:I12"/>
     <mergeCell ref="E13:I13"/>
     <mergeCell ref="E14:I14"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E18:I19"/>
-    <mergeCell ref="E20:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>